<commit_message>
Add file via upload
Modify the layout
</commit_message>
<xml_diff>
--- a/readme.xlsx
+++ b/readme.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA71868A-1A43-47AF-AF83-D7B76200947B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66FF37DE-133E-4811-B96C-CF78D2BC0732}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7200" xr2:uid="{E4450EF4-C089-4200-8C32-3721A0065C3F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11445" xr2:uid="{E4450EF4-C089-4200-8C32-3721A0065C3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="1" r:id="rId1"/>
@@ -2274,7 +2274,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D38A68B-9479-4008-8159-9542CB24F456}">
   <dimension ref="A1:A116"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <sheetData>
@@ -2343,7 +2343,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{317D7403-FF87-4A51-AC87-77B7823E196B}">
   <dimension ref="A1:A59"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <sheetData>
@@ -2402,7 +2402,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{728C3E59-169B-4492-9B24-1C584D91782D}">
   <dimension ref="A1:A66"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <sheetData>

</xml_diff>